<commit_message>
more datacamp and disk_savvy data
</commit_message>
<xml_diff>
--- a/datacamp.xlsx
+++ b/datacamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51980C3D-159F-4C45-A64A-3B3669BA7B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031D5807-DEB3-40A2-8B9C-1ADBB31BCE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Data Manipulation with pandas</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Introduction to NumPy</t>
+  </si>
+  <si>
+    <t>Intermediate SQL Queries</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -373,9 +376,10 @@
     <col min="3" max="4" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,8 +398,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -413,6 +420,9 @@
       </c>
       <c r="F2">
         <v>5</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more datacamp, disk_savvy and sullygnome data
</commit_message>
<xml_diff>
--- a/datacamp.xlsx
+++ b/datacamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54CAA2B-810B-496E-B980-63208BFC4E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D753B2-9BFB-4308-9828-59B4AA31C4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="5610" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="5610" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -691,7 +691,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,6 +873,9 @@
       <c r="C12">
         <v>4</v>
       </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">

</xml_diff>

<commit_message>
more datacamp and disk_savvy dara
</commit_message>
<xml_diff>
--- a/datacamp.xlsx
+++ b/datacamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F32A3-5385-4099-8C22-C2A5B07447FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344FD705-4CF5-4788-A54E-60E7D24C33D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="3375" windowWidth="7395" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="7395" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -937,7 +937,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,6 +1245,9 @@
       <c r="G12">
         <v>3</v>
       </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">

</xml_diff>

<commit_message>
moe datacamp and disk_savvy data
</commit_message>
<xml_diff>
--- a/datacamp.xlsx
+++ b/datacamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAF50AA-FF21-446B-BD7E-E77D0F4EDDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9163361-55CB-462D-94C1-321FE7273C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3930" windowWidth="7740" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="4275" windowWidth="7740" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1408,7 +1408,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,6 +1973,9 @@
       <c r="J19" s="2">
         <v>5</v>
       </c>
+      <c r="K19" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">

</xml_diff>